<commit_message>
created single file for pyinstaller
</commit_message>
<xml_diff>
--- a/PasswordRecords.xlsx
+++ b/PasswordRecords.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,18 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>5Paanwala-Hara</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Njolssss</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>